<commit_message>
Added sample for Charge Text
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/XSL-tmp/AlaskaCriminalCaseMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/XSL-tmp/AlaskaCriminalCaseMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="349">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -1062,6 +1062,24 @@
   </si>
   <si>
     <t>AK</t>
+  </si>
+  <si>
+    <t>      </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sec. 11.61.195. Misconduct involving weapons in the second degree. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>   (a) A person commits the crime of misconduct involving weapons in the second degree if the person knowingly   (1) possesses a firearm during the commission of an offense under AS 11.71.010 - 11.71.040;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1363,7 +1381,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1454,8 +1472,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1568,8 +1587,9 @@
     <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="90"/>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="91">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1655,6 +1675,7 @@
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -1960,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,11 +2714,13 @@
       </c>
       <c r="E53" s="26"/>
     </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="2" customFormat="1" ht="175.5" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="26"/>
+      <c r="B54" s="24" t="s">
+        <v>348</v>
+      </c>
       <c r="C54" s="26" t="s">
         <v>274</v>
       </c>
@@ -2708,8 +2731,8 @@
       <c r="A55" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="26">
-        <v>1</v>
+      <c r="B55" s="38" t="s">
+        <v>347</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>275</v>
@@ -3209,7 +3232,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
     </row>
-    <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
         <v>161</v>
       </c>
@@ -3460,8 +3483,11 @@
       <c r="I108" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B55" r:id="rId1" location="11.71.010" display="http://www.legis.state.ak.us/basis/statutes.asp - 11.71.010"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>